<commit_message>
Update GEVCU6 BOM, add parts list for GEVCU6, remove some ancient boards
</commit_message>
<xml_diff>
--- a/Shield/GEVCU-6_BOM.xlsx
+++ b/Shield/GEVCU-6_BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="GEVCU-6-2b" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,591 +20,627 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="195">
-  <si>
-    <t>Qty</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Device</t>
-  </si>
-  <si>
-    <t>Part Number</t>
-  </si>
-  <si>
-    <t>Vendor</t>
-  </si>
-  <si>
-    <t>Parts</t>
-  </si>
-  <si>
-    <t>Picture</t>
-  </si>
-  <si>
-    <t>GREEN</t>
-  </si>
-  <si>
-    <t>LED0805</t>
-  </si>
-  <si>
-    <t>645-598-8170-107F</t>
-  </si>
-  <si>
-    <t>Mouser</t>
-  </si>
-  <si>
-    <t>+3.3V, +5V, +12V, LED, USB2</t>
-  </si>
-  <si>
-    <t>10u</t>
-  </si>
-  <si>
-    <t>C-USC0805</t>
-  </si>
-  <si>
-    <t>80-C0805C106K8P</t>
-  </si>
-  <si>
-    <t>C1, C9, C11, C12, C22, C30, C33, C36, C39, C42, C53, C57, C66, C80, C82, C83, C85, C92, C94</t>
-  </si>
-  <si>
-    <t>0.1u</t>
-  </si>
-  <si>
-    <t>80-C0805C104J8R</t>
-  </si>
-  <si>
-    <t>C2, C3, C4, C5, C6, C7, C8, C10, C13, C14, C15, C16, C17, C18, C19, C20, C21, C29, C31, C32, C34, C35, C37, C38, C40, C41, C46, C49, C52, C55, C56, C61, C64, C65, C67, C68, C70, C71, C73, C76, C79, C81, C87, C90, C91, C95</t>
-  </si>
-  <si>
-    <t>22p</t>
-  </si>
-  <si>
-    <t>C-USC1206</t>
-  </si>
-  <si>
-    <t>77-VJ1206A220JXQCBC</t>
-  </si>
-  <si>
-    <t>C23, C24, C54</t>
-  </si>
-  <si>
-    <t>581-0805ZA220JAT2A</t>
-  </si>
-  <si>
-    <t>C25, C26, C27</t>
-  </si>
-  <si>
-    <t>0.01u</t>
-  </si>
-  <si>
-    <t>77-VJ0805A103KXQTBC</t>
-  </si>
-  <si>
-    <t>C28</t>
-  </si>
-  <si>
-    <t>0.033u</t>
-  </si>
-  <si>
-    <t>77-VJ0805Y333KBABC31</t>
-  </si>
-  <si>
-    <t>C43, C44, C45, C50, C51, C58, C59, C60, C84, C86</t>
-  </si>
-  <si>
-    <t>4.7u</t>
-  </si>
-  <si>
-    <t>810-CGA4J1X7R1E475MA</t>
-  </si>
-  <si>
-    <t>C47, C48, C62, C63, C88, C89</t>
-  </si>
-  <si>
-    <t>47n</t>
-  </si>
-  <si>
-    <t>581-0805ZC473JAZ2A</t>
-  </si>
-  <si>
-    <t>C69, C72</t>
-  </si>
-  <si>
-    <t>100u</t>
-  </si>
-  <si>
-    <t>CPOL-USE2.5-6</t>
-  </si>
-  <si>
-    <t>667-EEU-FM1E101</t>
-  </si>
-  <si>
-    <t>C74</t>
-  </si>
-  <si>
-    <t>1u</t>
-  </si>
-  <si>
-    <t>80-C0805C105J3RACTU</t>
-  </si>
-  <si>
-    <t>C75, C93</t>
-  </si>
-  <si>
-    <t>2u</t>
-  </si>
-  <si>
-    <t>810-CGA4J1X7R1V225K</t>
-  </si>
-  <si>
-    <t>C77</t>
-  </si>
-  <si>
-    <t>0.01u 2kv</t>
-  </si>
-  <si>
-    <t>C-USC1812</t>
-  </si>
-  <si>
-    <t>605-202S43W103KV4E</t>
-  </si>
-  <si>
-    <t>C78</t>
-  </si>
-  <si>
-    <t>680u</t>
-  </si>
-  <si>
-    <t>CPOL-US5-10.5</t>
-  </si>
-  <si>
-    <t>661-EKZM250E681MJ16S</t>
-  </si>
-  <si>
-    <t>C96</t>
-  </si>
-  <si>
-    <t>MBR0520LT</t>
-  </si>
-  <si>
-    <t>512-MBR0520L</t>
-  </si>
-  <si>
-    <t>D1, D2, D3, D4, D5, D6, D7, D8</t>
-  </si>
-  <si>
-    <t>B360B-13-F</t>
-  </si>
-  <si>
-    <t>DIODE-SMB</t>
-  </si>
-  <si>
-    <t>621-B360B-F</t>
-  </si>
-  <si>
-    <t>D9</t>
-  </si>
-  <si>
-    <t>BAS70XY</t>
-  </si>
-  <si>
-    <t>771-BAS70XY115</t>
-  </si>
-  <si>
-    <t>D10, D11, D12, D13, D14, D20, D36</t>
-  </si>
-  <si>
-    <t>PUCHBUTTON</t>
-  </si>
-  <si>
-    <t>PUSHBUTTON</t>
-  </si>
-  <si>
-    <t>688-SKQYAB</t>
-  </si>
-  <si>
-    <t>ERASE, RESET</t>
-  </si>
-  <si>
-    <t>ISO1050DW</t>
-  </si>
-  <si>
-    <t>ISO1050</t>
-  </si>
-  <si>
-    <t>595-ISO1050DW</t>
-  </si>
-  <si>
-    <t>IC9, IC10</t>
-  </si>
-  <si>
-    <t>1x18HEADER</t>
-  </si>
-  <si>
-    <t>PINHD_1x18</t>
-  </si>
-  <si>
-    <t>517-929850-01-18-RA</t>
-  </si>
-  <si>
-    <t>JP1, JP2</t>
-  </si>
-  <si>
-    <t>MH2029-300Y</t>
-  </si>
-  <si>
-    <t>WE-CBF_0805</t>
-  </si>
-  <si>
-    <t>652-MH2029-300Y</t>
-  </si>
-  <si>
-    <t>L1, L2, L3, L4, L5, L6, L7, L8, L9, L10, L11, L12, L13</t>
-  </si>
-  <si>
-    <t>ILD213</t>
-  </si>
-  <si>
-    <t>782-ILD213T</t>
-  </si>
-  <si>
-    <t>OK1, OK2</t>
-  </si>
-  <si>
-    <t>2.5A</t>
-  </si>
-  <si>
-    <t>PTC1812</t>
-  </si>
-  <si>
-    <t>576-1812L150/12DR</t>
-  </si>
-  <si>
-    <t>PTC, PTC0, PTC1, PTC2, PTC3, PTC4, PTC5, PTC6, PTC7</t>
-  </si>
-  <si>
-    <t>100k</t>
-  </si>
-  <si>
-    <t>R-US_R0805</t>
-  </si>
-  <si>
-    <t>71-CRCW0805J-100K-E3</t>
-  </si>
-  <si>
-    <t>R1, R24, R28, R29, R30</t>
-  </si>
-  <si>
-    <t>39R 1%</t>
-  </si>
-  <si>
-    <t>71-CRCW0805-39</t>
-  </si>
-  <si>
-    <t>R2, R3</t>
-  </si>
-  <si>
-    <t>6k8 1%</t>
-  </si>
-  <si>
-    <t>71-CRCW0805-6.8K-E3</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>402R</t>
-  </si>
-  <si>
-    <t>71-CRCW0805-402-E3</t>
-  </si>
-  <si>
-    <t>R5, R58</t>
-  </si>
-  <si>
-    <t>10R</t>
-  </si>
-  <si>
-    <t>667-ERJ-6GEYJ100V</t>
-  </si>
-  <si>
-    <t>R6, R7, R8, R9, R74, R75, R76, R77</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>667-ERJ-6GEYJ103V</t>
-  </si>
-  <si>
-    <t>R10, R14, R17, R21, R27, R42, R43, R48, R49, R66, R67, R68, R69, R70, R71, R72, R73</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>71-RCG08051K00JNEA</t>
-  </si>
-  <si>
-    <t>R11, R12, R13, R15, R16, R18, R19, R20, R44, R45, R46, R47, R50, R51, R52, R53, R57, R65</t>
-  </si>
-  <si>
-    <t>1M</t>
-  </si>
-  <si>
-    <t>R-US_R1206</t>
-  </si>
-  <si>
-    <t>71-TNPV12061M00BEEN</t>
-  </si>
-  <si>
-    <t>R22, R26</t>
-  </si>
-  <si>
-    <t>2K</t>
-  </si>
-  <si>
-    <t>279-RP73PF2A2K0BTDF</t>
-  </si>
-  <si>
-    <t>R23, R25</t>
-  </si>
-  <si>
-    <t>60R</t>
-  </si>
-  <si>
-    <t>667-ERJ-P06D60R4V</t>
-  </si>
-  <si>
-    <t>R38, R39, R40, R41</t>
-  </si>
-  <si>
-    <t>4.7k</t>
-  </si>
-  <si>
-    <t>71-CRCW0805J-4.7K-E3</t>
-  </si>
-  <si>
-    <t>R54, R55</t>
-  </si>
-  <si>
-    <t>3k3</t>
-  </si>
-  <si>
-    <t>660-RK73G2ATTD3301F</t>
-  </si>
-  <si>
-    <t>R56</t>
-  </si>
-  <si>
-    <t>NMOSSOT223</t>
-  </si>
-  <si>
-    <t>726-BSP295H6327XTSA1</t>
-  </si>
-  <si>
-    <t>T2, T4, T5, T6, T7, T8, T10, T12</t>
-  </si>
-  <si>
-    <t>SMBJ15A-TR</t>
-  </si>
-  <si>
-    <t>SUPPRESSOR_SMB</t>
-  </si>
-  <si>
-    <t>511-SMBJ15A</t>
-  </si>
-  <si>
-    <t>TVS</t>
-  </si>
-  <si>
-    <t>CINCON5V</t>
-  </si>
-  <si>
-    <t>Tracor </t>
-  </si>
-  <si>
-    <t>TMR 6-2411WI </t>
-  </si>
-  <si>
-    <t>U$1</t>
-  </si>
-  <si>
-    <t>581_01_48_005_S</t>
-  </si>
-  <si>
-    <t>581-01-48-005</t>
-  </si>
-  <si>
-    <t>U$2</t>
-  </si>
-  <si>
-    <t>ASE</t>
-  </si>
-  <si>
-    <t>788-8103AI233E-4.0X</t>
-  </si>
-  <si>
-    <t>U$3</t>
-  </si>
-  <si>
-    <t>ATSAM3X8EA-AU</t>
-  </si>
-  <si>
-    <t>ATSAM3X</t>
-  </si>
-  <si>
-    <t>556-ATSAM3X8EA-AU</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>ADUM3221BRZ</t>
-  </si>
-  <si>
-    <t>ADUM3221</t>
-  </si>
-  <si>
-    <t>584-ADUM3221BRZ</t>
-  </si>
-  <si>
-    <t>U3, U4, U5, U6</t>
-  </si>
-  <si>
-    <t>M24M02-DRMN6TP</t>
-  </si>
-  <si>
-    <t>EEPROM</t>
-  </si>
-  <si>
-    <t>511-M24M02-DRMN6TP</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
-    <t>TRACO</t>
-  </si>
-  <si>
-    <t>TEL5-1210</t>
-  </si>
-  <si>
-    <t>Powergate</t>
-  </si>
-  <si>
-    <t>U8</t>
-  </si>
-  <si>
-    <t>TSR-1</t>
-  </si>
-  <si>
-    <t>TSR1-2450</t>
-  </si>
-  <si>
-    <t>U9</t>
-  </si>
-  <si>
-    <t>LM1117</t>
-  </si>
-  <si>
-    <t>926-LM1117IMPX33NOPB</t>
-  </si>
-  <si>
-    <t>U10</t>
-  </si>
-  <si>
-    <t>ADE7913</t>
-  </si>
-  <si>
-    <t>584-ADE7913ARIZ</t>
-  </si>
-  <si>
-    <t>U11, U12, U24</t>
-  </si>
-  <si>
-    <t>PN61729-S</t>
-  </si>
-  <si>
-    <t>PN61729</t>
-  </si>
-  <si>
-    <t>292304-1</t>
-  </si>
-  <si>
-    <t>X1</t>
-  </si>
-  <si>
-    <t>12MHz </t>
-  </si>
-  <si>
-    <t>CRYSTAL-3.2x2.5</t>
-  </si>
-  <si>
-    <t>520-120-20-33-CKMT</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>32.768Khz</t>
-  </si>
-  <si>
-    <t>732-FC135-32.76KAAC3</t>
-  </si>
-  <si>
-    <t>1SMB5929BT3G</t>
-  </si>
-  <si>
-    <t>ZENER-DIODESMB</t>
-  </si>
-  <si>
-    <t>863-1SMB5929BT3G</t>
-  </si>
-  <si>
-    <t>ZEN</t>
-  </si>
-  <si>
-    <t>2x10 Header</t>
-  </si>
-  <si>
-    <t>2x10 1.27mm Header</t>
-  </si>
-  <si>
-    <t>855-M50-3500542</t>
-  </si>
-  <si>
-    <t>JTAG</t>
-  </si>
-  <si>
-    <t>Parts not placed onto PCB:</t>
-  </si>
-  <si>
-    <t>18ga pins for cinch plug</t>
-  </si>
-  <si>
-    <t>538-425-00-00-873</t>
-  </si>
-  <si>
-    <t>30 pin plug for 48 pin enclosure</t>
-  </si>
-  <si>
-    <t>538-581-01-30-029</t>
-  </si>
-  <si>
-    <t>18 pin plug for 48 pin enclosure</t>
-  </si>
-  <si>
-    <t>538-581-01-18-023</t>
-  </si>
-  <si>
-    <t>MODICE Enclosure</t>
-  </si>
-  <si>
-    <t>538-581-01-30-043</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="207">
+  <si>
+    <t xml:space="preserve">Qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Picture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GREEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">645-598-8170-107F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mouser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+3.3V, +5V, +12V, LED, USB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C-USC0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80-C0805C106K8P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1, C9, C11, C12, C22, C30, C33, C36, C39, C42, C53, C57, C66, C80, C82, C83, C85, C92, C94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80-C0805C104J8R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2, C3, C4, C5, C6, C7, C8, C10, C13, C14, C15, C16, C17, C18, C19, C20, C21, C29, C31, C32, C34, C35, C37, C38, C40, C41, C43, C44, C45, C46, C49, C52, C55, C56, C58, C59, C60, C61, C64, C65, C67, C68, C70, C71, C73, C76, C79, C81, C84, C86, C87, C90, C91, C95, C97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C-USC1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77-VJ1206A220JXQCBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C23, C24, C54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">581-0805ZA220JAT2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C25, C26, C27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77-VJ0805A103KXQTBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.033u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77-VJ0805Y333KBABC31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C50, C51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.7u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">810-CGA4J1X7R1E475MA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C47, C48, C62, C63, C88, C89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">581-0805ZC473JAZ2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C69, C72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPOL-USE2.5-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-EEU-FM1E101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80-C0805C105J3RACTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C75, C93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">810-CGA4J1X7R1V225K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01u 2kv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C-USC1812</t>
+  </si>
+  <si>
+    <t xml:space="preserve">605-202S43W103KV4E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">680u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPOL-US5-10.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">661-EKZM250E681MJ16S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBR0520LT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">512-MBR0520L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1, D2, D3, D4, D5, D6, D7, D8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B360B-13-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIODE-SMB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">621-B360B-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAS70XY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">771-BAS70XY115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D10, D11, D12, D13, D14, D20, D36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUCHBUTTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUSHBUTTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">688-SKQYAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERASE, RESET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISO1050DW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISO1050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">595-ISO1050DW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC9, IC10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x18HEADER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PINHD_1x18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">517-929850-01-18-RA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JP1, JP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MH2029-300Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WE-CBF_0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">652-MH2029-300Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1, L2, L3, L4, L5, L6, L7, L8, L9, L10, L11, L12, L13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILD213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">782-ILD213T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK1, OK2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTC1812</t>
+  </si>
+  <si>
+    <t xml:space="preserve">576-1812L150/12DR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTC, PTC0, PTC1, PTC2, PTC3, PTC4, PTC5, PTC6, PTC7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R-US_R0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71-CRCW0805J-100K-E3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1, R24, R28, R29, R30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39R 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71-CRCW0805-39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2, R3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6k8 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71-CRCW0805-6.8K-E3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">402R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71-CRCW0805-402-E3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5, R58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-6GEYJ100V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6, R7, R8, R9, R74, R75, R76, R77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-6GEYJ103V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R27, R42, R43, R48, R49, R66, R67, R68, R69, R70, R71, R72, R73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14k 0.1% Thin Film</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERA-6AEB1402V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R10, R14, R17, R21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71-RCG08051K00JNEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R44, R45, R46, R47, R50, R51, R52, R53, R57, R65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1k 0.1% Thin film</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERA-6AEB102V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R11, R13, R15, R18, R20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1M 0.1% Thin Film (300V)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R-US_R1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">279-CPF1206B1M0E1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R22, R26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 Ohm Thin Film</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603-AF0805JR-070RL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R12, R19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">750R 0.1% Thin Film</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERA-6AEB751V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5k 0.1% Thin Film</t>
+  </si>
+  <si>
+    <t xml:space="preserve">279-CPF0805B1K5E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R23, R25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-P06D60R4V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R38, R39, R40, R41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.7k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71-CRCW0805J-4.7K-E3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R54, R55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3k3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">660-RK73G2ATTD3301F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMOSSOT223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">726-BSP295H6327XTSA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T2, T4, T5, T6, T7, T8, T10, T12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMBJ15A-TR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUPPRESSOR_SMB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">511-SMBJ15A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TVS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CINCON5V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tracor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMR 6-2411WI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">U$1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">581_01_48_005_S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">581-01-48-005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U$2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">788-8103AI233E-4.0X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U$3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATSAM3X8EA-AU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATSAM3X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">556-ATSAM3X8EA-AU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADUM3221BRZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADUM3221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">584-ADUM3221BRZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U3, U4, U5, U6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M24M02-DRMN6TP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EEPROM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">511-M24M02-DRMN6TP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRACO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEL5-1210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Powergate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSR-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSR1-2450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LM1117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">926-LM1117IMPX33NOPB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADE7913</t>
+  </si>
+  <si>
+    <t xml:space="preserve">584-ADE7913ARIZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U11, U12, U24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PN61729-S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PN61729</t>
+  </si>
+  <si>
+    <t xml:space="preserve">292304-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12MHz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRYSTAL-3.2x2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">520-120-20-33-CKMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32.768Khz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">732-FC135-32.76KAAC3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1SMB5929BT3G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZENER-DIODESMB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">863-1SMB5929BT3G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x10 Header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x10 1.27mm Header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">855-M50-3500542</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JTAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parts not placed onto PCB:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18ga pins for cinch plug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">538-425-00-00-873</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 pin plug for 48 pin enclosure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">538-581-01-30-029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 pin plug for 48 pin enclosure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">538-581-01-18-023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MODICE Enclosure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">538-581-01-30-043</t>
   </si>
 </sst>
 </file>
@@ -612,7 +648,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -776,8 +812,8 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -824,7 +860,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -840,9 +876,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>522720</xdr:colOff>
+      <xdr:colOff>522360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>349920</xdr:rowOff>
+      <xdr:rowOff>349560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -855,8 +891,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9609120" y="381240"/>
-          <a:ext cx="447840" cy="349560"/>
+          <a:off x="9995400" y="381240"/>
+          <a:ext cx="447480" cy="349200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -873,13 +909,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>74880</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>11880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>493560</xdr:colOff>
+      <xdr:colOff>493200</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>372240</xdr:rowOff>
+      <xdr:rowOff>373320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -892,8 +928,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9609120" y="772200"/>
-          <a:ext cx="418680" cy="361800"/>
+          <a:off x="9995400" y="773640"/>
+          <a:ext cx="418320" cy="361440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -914,9 +950,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>503280</xdr:colOff>
+      <xdr:colOff>502920</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>361800</xdr:rowOff>
+      <xdr:rowOff>361440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -929,8 +965,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9618840" y="1143360"/>
-          <a:ext cx="418680" cy="361440"/>
+          <a:off x="10005120" y="1143360"/>
+          <a:ext cx="418320" cy="361080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -951,9 +987,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>480240</xdr:colOff>
+      <xdr:colOff>479880</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>315000</xdr:rowOff>
+      <xdr:rowOff>314640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -966,8 +1002,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9609120" y="1562400"/>
-          <a:ext cx="405360" cy="276480"/>
+          <a:off x="9995400" y="1562400"/>
+          <a:ext cx="405000" cy="276120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -984,13 +1020,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>74880</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>30960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>465840</xdr:colOff>
+      <xdr:colOff>465480</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>314280</xdr:rowOff>
+      <xdr:rowOff>315360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1003,8 +1039,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9609120" y="1934280"/>
-          <a:ext cx="390960" cy="284760"/>
+          <a:off x="9995400" y="1935720"/>
+          <a:ext cx="390600" cy="284400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1025,9 +1061,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>447120</xdr:colOff>
+      <xdr:colOff>446760</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>273240</xdr:rowOff>
+      <xdr:rowOff>272880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1040,8 +1076,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9609120" y="2305440"/>
-          <a:ext cx="372240" cy="253800"/>
+          <a:off x="9995400" y="2305440"/>
+          <a:ext cx="371880" cy="253440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1062,9 +1098,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>425880</xdr:colOff>
+      <xdr:colOff>425520</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>301320</xdr:rowOff>
+      <xdr:rowOff>300960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1077,8 +1113,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9618840" y="2715120"/>
-          <a:ext cx="341280" cy="253080"/>
+          <a:off x="10005120" y="2715120"/>
+          <a:ext cx="340920" cy="252720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1095,13 +1131,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>74880</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>11880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>495000</xdr:colOff>
+      <xdr:colOff>494640</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>353160</xdr:rowOff>
+      <xdr:rowOff>354240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1114,8 +1150,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9609120" y="3058200"/>
-          <a:ext cx="420120" cy="342720"/>
+          <a:off x="9995400" y="3059640"/>
+          <a:ext cx="419760" cy="342360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1136,9 +1172,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>456480</xdr:colOff>
+      <xdr:colOff>456120</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>333000</xdr:rowOff>
+      <xdr:rowOff>332640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1151,8 +1187,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9599760" y="3439080"/>
-          <a:ext cx="390960" cy="322920"/>
+          <a:off x="9986040" y="3439080"/>
+          <a:ext cx="390600" cy="322560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1173,9 +1209,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>435960</xdr:colOff>
+      <xdr:colOff>435600</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>315360</xdr:rowOff>
+      <xdr:rowOff>315000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1188,8 +1224,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9666360" y="3858120"/>
-          <a:ext cx="303840" cy="267120"/>
+          <a:off x="10052640" y="3858120"/>
+          <a:ext cx="303480" cy="266760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1206,13 +1242,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>74880</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:rowOff>21240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>522360</xdr:colOff>
+      <xdr:colOff>522000</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>362520</xdr:rowOff>
+      <xdr:rowOff>363600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1225,8 +1261,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9609120" y="4210560"/>
-          <a:ext cx="447480" cy="342720"/>
+          <a:off x="9995400" y="4212000"/>
+          <a:ext cx="447120" cy="342360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1247,9 +1283,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>451800</xdr:colOff>
+      <xdr:colOff>451440</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>321840</xdr:rowOff>
+      <xdr:rowOff>321480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1262,8 +1298,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9657000" y="4591440"/>
-          <a:ext cx="329040" cy="302400"/>
+          <a:off x="10043280" y="4591440"/>
+          <a:ext cx="328680" cy="302040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1284,9 +1320,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>458640</xdr:colOff>
+      <xdr:colOff>458280</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>333360</xdr:rowOff>
+      <xdr:rowOff>333000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1299,8 +1335,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9647280" y="4953240"/>
-          <a:ext cx="345600" cy="333000"/>
+          <a:off x="10033560" y="4953240"/>
+          <a:ext cx="345240" cy="332640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1317,13 +1353,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>84600</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>38880</xdr:rowOff>
+      <xdr:rowOff>40320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>464040</xdr:colOff>
+      <xdr:colOff>463680</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>304560</xdr:rowOff>
+      <xdr:rowOff>305640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1336,8 +1372,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9618840" y="5372640"/>
-          <a:ext cx="379440" cy="265680"/>
+          <a:off x="10005120" y="5374080"/>
+          <a:ext cx="379080" cy="265320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1358,9 +1394,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>507600</xdr:colOff>
+      <xdr:colOff>507240</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>314280</xdr:rowOff>
+      <xdr:rowOff>313920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1373,8 +1409,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9570960" y="5734440"/>
-          <a:ext cx="470880" cy="294840"/>
+          <a:off x="9957240" y="5734440"/>
+          <a:ext cx="470520" cy="294480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1395,9 +1431,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>473400</xdr:colOff>
+      <xdr:colOff>473040</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>343800</xdr:rowOff>
+      <xdr:rowOff>343440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1410,8 +1446,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9618840" y="6105960"/>
-          <a:ext cx="388800" cy="333720"/>
+          <a:off x="10005120" y="6105960"/>
+          <a:ext cx="388440" cy="333360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1428,13 +1464,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>84600</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>11880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>469800</xdr:colOff>
+      <xdr:colOff>469440</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>325080</xdr:rowOff>
+      <xdr:rowOff>326160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1447,8 +1483,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9618840" y="6487200"/>
-          <a:ext cx="385200" cy="314640"/>
+          <a:off x="10005120" y="6488640"/>
+          <a:ext cx="384840" cy="314280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1469,9 +1505,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>464040</xdr:colOff>
+      <xdr:colOff>463680</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>324000</xdr:rowOff>
+      <xdr:rowOff>323640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1484,8 +1520,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9618840" y="6868080"/>
-          <a:ext cx="379440" cy="313920"/>
+          <a:off x="10005120" y="6868080"/>
+          <a:ext cx="379080" cy="313560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1506,9 +1542,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>497520</xdr:colOff>
+      <xdr:colOff>497160</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>352440</xdr:rowOff>
+      <xdr:rowOff>352080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1521,8 +1557,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9609120" y="7258320"/>
-          <a:ext cx="422640" cy="333000"/>
+          <a:off x="9995400" y="7258320"/>
+          <a:ext cx="422280" cy="332640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1539,13 +1575,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>55800</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>30960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>465120</xdr:colOff>
+      <xdr:colOff>464760</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>339840</xdr:rowOff>
+      <xdr:rowOff>340920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1558,8 +1594,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9590040" y="7649280"/>
-          <a:ext cx="409320" cy="310320"/>
+          <a:off x="9976320" y="7650720"/>
+          <a:ext cx="408960" cy="309960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1580,9 +1616,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>550800</xdr:colOff>
+      <xdr:colOff>550440</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>322920</xdr:rowOff>
+      <xdr:rowOff>322560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1595,8 +1631,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9609120" y="8068320"/>
-          <a:ext cx="475920" cy="255600"/>
+          <a:off x="9995400" y="8068320"/>
+          <a:ext cx="475560" cy="255240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1617,9 +1653,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>436680</xdr:colOff>
+      <xdr:colOff>436320</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>346320</xdr:rowOff>
+      <xdr:rowOff>345960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1632,8 +1668,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9666360" y="8391960"/>
-          <a:ext cx="304560" cy="336240"/>
+          <a:off x="10052640" y="8391960"/>
+          <a:ext cx="304200" cy="335880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1650,13 +1686,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>74880</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>11880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>493560</xdr:colOff>
+      <xdr:colOff>493200</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>362520</xdr:rowOff>
+      <xdr:rowOff>363600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1669,8 +1705,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9609120" y="8773200"/>
-          <a:ext cx="418680" cy="352080"/>
+          <a:off x="9995400" y="8774640"/>
+          <a:ext cx="418320" cy="351720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1691,9 +1727,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>510120</xdr:colOff>
+      <xdr:colOff>509760</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>342360</xdr:rowOff>
+      <xdr:rowOff>342000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1706,8 +1742,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9599760" y="9154080"/>
-          <a:ext cx="444600" cy="332280"/>
+          <a:off x="9986040" y="9154080"/>
+          <a:ext cx="444240" cy="331920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1728,9 +1764,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>519480</xdr:colOff>
+      <xdr:colOff>519120</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>342360</xdr:rowOff>
+      <xdr:rowOff>342000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1743,8 +1779,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9609120" y="9534960"/>
-          <a:ext cx="444600" cy="332280"/>
+          <a:off x="9995400" y="9534960"/>
+          <a:ext cx="444240" cy="331920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1761,13 +1797,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>65520</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>11880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>510120</xdr:colOff>
+      <xdr:colOff>509760</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
+      <xdr:rowOff>343800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1780,8 +1816,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9599760" y="9916200"/>
-          <a:ext cx="444600" cy="332280"/>
+          <a:off x="9986040" y="9917640"/>
+          <a:ext cx="444240" cy="331920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1802,9 +1838,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>510120</xdr:colOff>
+      <xdr:colOff>509760</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>351720</xdr:rowOff>
+      <xdr:rowOff>351360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1817,8 +1853,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9599760" y="10306440"/>
-          <a:ext cx="444600" cy="332280"/>
+          <a:off x="9986040" y="10306440"/>
+          <a:ext cx="444240" cy="331920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1839,9 +1875,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>538560</xdr:colOff>
+      <xdr:colOff>538200</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>342360</xdr:rowOff>
+      <xdr:rowOff>342000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1854,8 +1890,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9628200" y="10677960"/>
-          <a:ext cx="444600" cy="332280"/>
+          <a:off x="10014480" y="10677960"/>
+          <a:ext cx="444240" cy="331920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1872,13 +1908,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>74880</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>2160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>519480</xdr:colOff>
+      <xdr:colOff>519120</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>333000</xdr:rowOff>
+      <xdr:rowOff>334080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1891,8 +1927,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9609120" y="11049480"/>
-          <a:ext cx="444600" cy="332280"/>
+          <a:off x="9995400" y="11050920"/>
+          <a:ext cx="444240" cy="331920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1908,14 +1944,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>132120</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>29160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>446760</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>331200</xdr:rowOff>
+      <xdr:colOff>446400</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>330840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1928,8 +1964,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9666360" y="11459160"/>
-          <a:ext cx="314640" cy="302040"/>
+          <a:off x="10052640" y="11840040"/>
+          <a:ext cx="314280" cy="301680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1945,13 +1981,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>55800</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>493560</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:colOff>493200</xdr:colOff>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>327600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1965,8 +2001,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9590040" y="11830320"/>
-          <a:ext cx="437760" cy="308160"/>
+          <a:off x="9976320" y="12592800"/>
+          <a:ext cx="437400" cy="307800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1982,14 +2018,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>113040</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>10440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>493560</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>347400</xdr:rowOff>
+      <xdr:colOff>493200</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>347040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2002,8 +2038,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9647280" y="12202200"/>
-          <a:ext cx="380520" cy="336960"/>
+          <a:off x="10033560" y="14107320"/>
+          <a:ext cx="380160" cy="336600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2019,14 +2055,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>46440</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>478440</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>295200</xdr:rowOff>
+      <xdr:colOff>478080</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>295560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2039,8 +2075,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9580680" y="12592440"/>
-          <a:ext cx="432000" cy="275760"/>
+          <a:off x="9966960" y="14117040"/>
+          <a:ext cx="431640" cy="275400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2056,14 +2092,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>65520</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>510120</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>351720</xdr:rowOff>
+      <xdr:colOff>509760</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>352080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2076,8 +2112,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9599760" y="12973320"/>
-          <a:ext cx="444600" cy="332280"/>
+          <a:off x="9986040" y="14497920"/>
+          <a:ext cx="444240" cy="331920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2093,14 +2129,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>36720</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>19800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>481320</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>352080</xdr:rowOff>
+      <xdr:colOff>480960</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>351720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2113,8 +2149,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9570960" y="13354560"/>
-          <a:ext cx="444600" cy="332280"/>
+          <a:off x="9957240" y="14878800"/>
+          <a:ext cx="444240" cy="331920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2130,14 +2166,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>84600</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>459360</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>343080</xdr:rowOff>
+      <xdr:colOff>459000</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>343440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2150,8 +2186,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9618840" y="13745160"/>
-          <a:ext cx="374760" cy="313920"/>
+          <a:off x="10005120" y="15269760"/>
+          <a:ext cx="374400" cy="313560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2167,14 +2203,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>55800</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>10800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>522000</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>357120</xdr:rowOff>
+      <xdr:colOff>521640</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>357480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2187,8 +2223,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9590040" y="14106960"/>
-          <a:ext cx="466200" cy="347040"/>
+          <a:off x="9976320" y="15631560"/>
+          <a:ext cx="465840" cy="346680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2204,14 +2240,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>84600</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>29520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>484200</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>341640</xdr:rowOff>
+      <xdr:colOff>483840</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>341280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2224,8 +2260,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9618840" y="14507280"/>
-          <a:ext cx="399600" cy="312120"/>
+          <a:off x="10005120" y="16031520"/>
+          <a:ext cx="399240" cy="311760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2241,14 +2277,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>46440</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>550800</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>352800</xdr:rowOff>
+      <xdr:colOff>550440</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>353160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2261,8 +2297,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9580680" y="14888160"/>
-          <a:ext cx="504360" cy="323640"/>
+          <a:off x="9966960" y="16412760"/>
+          <a:ext cx="504000" cy="323280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2278,14 +2314,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>113040</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>506520</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>333360</xdr:rowOff>
+      <xdr:colOff>506160</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>333720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2298,8 +2334,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9647280" y="15259320"/>
-          <a:ext cx="393480" cy="313920"/>
+          <a:off x="10033560" y="16783920"/>
+          <a:ext cx="393120" cy="313560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2315,14 +2351,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>122760</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>10440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>494640</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>364320</xdr:rowOff>
+      <xdr:colOff>494280</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>363960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2335,8 +2371,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9657000" y="15631200"/>
-          <a:ext cx="371880" cy="353880"/>
+          <a:off x="10043280" y="17155440"/>
+          <a:ext cx="371520" cy="353520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2352,14 +2388,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>160560</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>10800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>467640</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>333720</xdr:rowOff>
+      <xdr:colOff>467280</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>334080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2372,8 +2408,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9694800" y="16012080"/>
-          <a:ext cx="307080" cy="323640"/>
+          <a:off x="10081080" y="17536680"/>
+          <a:ext cx="306720" cy="323280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2389,14 +2425,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>79920</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>67320</xdr:rowOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>484560</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>315720</xdr:rowOff>
+      <xdr:colOff>484200</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>316080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2409,8 +2445,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9614160" y="16450200"/>
-          <a:ext cx="404640" cy="248400"/>
+          <a:off x="10000440" y="17974800"/>
+          <a:ext cx="404280" cy="248040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2426,14 +2462,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>103680</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>10440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>517320</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>315000</xdr:rowOff>
+      <xdr:colOff>516960</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>314640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2446,8 +2482,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9637920" y="16774200"/>
-          <a:ext cx="413640" cy="304560"/>
+          <a:off x="10024200" y="18298440"/>
+          <a:ext cx="413280" cy="304200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2463,14 +2499,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>141840</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>474840</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>333360</xdr:rowOff>
+      <xdr:colOff>474480</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>333720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2483,8 +2519,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9676080" y="17145360"/>
-          <a:ext cx="333000" cy="333000"/>
+          <a:off x="10062360" y="18669960"/>
+          <a:ext cx="332640" cy="332640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2500,14 +2536,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>103680</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>474840</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>343080</xdr:rowOff>
+      <xdr:colOff>474480</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>343440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2520,8 +2556,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9637920" y="17555040"/>
-          <a:ext cx="371160" cy="313920"/>
+          <a:off x="10024200" y="19079640"/>
+          <a:ext cx="370800" cy="313560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2537,14 +2573,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>74880</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>29520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>465120</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>320760</xdr:rowOff>
+      <xdr:colOff>464760</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>320400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2557,8 +2593,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9609120" y="17936280"/>
-          <a:ext cx="390240" cy="291240"/>
+          <a:off x="9995400" y="19460520"/>
+          <a:ext cx="389880" cy="290880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2574,14 +2610,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>113040</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>10800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>407880</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>309600</xdr:rowOff>
+      <xdr:colOff>407520</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>309960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2594,8 +2630,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9647280" y="18298080"/>
-          <a:ext cx="294840" cy="299520"/>
+          <a:off x="10033560" y="19822680"/>
+          <a:ext cx="294480" cy="299160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2611,14 +2647,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>122760</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>10800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>417600</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>349920</xdr:rowOff>
+      <xdr:colOff>417240</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>350280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2631,8 +2667,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9657000" y="18298080"/>
-          <a:ext cx="294840" cy="339840"/>
+          <a:off x="10043280" y="19822680"/>
+          <a:ext cx="294480" cy="339480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2648,14 +2684,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>84600</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>475560</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>324000</xdr:rowOff>
+      <xdr:colOff>475200</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>324360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2668,8 +2704,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9618840" y="18688320"/>
-          <a:ext cx="390960" cy="304560"/>
+          <a:off x="10005120" y="20212920"/>
+          <a:ext cx="390600" cy="304200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2685,14 +2721,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>74880</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>19800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>474480</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>342000</xdr:rowOff>
+      <xdr:colOff>474120</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>341640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2705,8 +2741,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9609120" y="19069560"/>
-          <a:ext cx="399600" cy="322200"/>
+          <a:off x="9995400" y="20593800"/>
+          <a:ext cx="399240" cy="321840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2722,14 +2758,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>103680</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>528840</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>343800</xdr:rowOff>
+      <xdr:colOff>528480</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>344160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2742,8 +2778,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9637920" y="19841040"/>
-          <a:ext cx="425160" cy="314640"/>
+          <a:off x="10024200" y="21365640"/>
+          <a:ext cx="424800" cy="314280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2759,14 +2795,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>113040</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>466920</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>304920</xdr:rowOff>
+      <xdr:colOff>466560</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>305280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2779,8 +2815,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9647280" y="19431360"/>
-          <a:ext cx="353880" cy="304560"/>
+          <a:off x="10033560" y="20955960"/>
+          <a:ext cx="353520" cy="304200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2796,14 +2832,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>84600</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>498240</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>314640</xdr:rowOff>
+      <xdr:colOff>497880</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>315720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2816,8 +2852,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9618840" y="20747880"/>
-          <a:ext cx="413640" cy="285480"/>
+          <a:off x="10005120" y="22273200"/>
+          <a:ext cx="413280" cy="285120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2833,14 +2869,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>65520</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>29520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>484920</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>328320</xdr:rowOff>
+      <xdr:colOff>484560</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>327960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2853,8 +2889,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9599760" y="21090960"/>
-          <a:ext cx="419400" cy="298800"/>
+          <a:off x="9986040" y="22615200"/>
+          <a:ext cx="419040" cy="298440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2870,14 +2906,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>65520</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>451080</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>304920</xdr:rowOff>
+      <xdr:colOff>450720</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>306000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2890,8 +2926,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9599760" y="21404880"/>
-          <a:ext cx="385560" cy="304560"/>
+          <a:off x="9986040" y="22930200"/>
+          <a:ext cx="385200" cy="304200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2907,14 +2943,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>46440</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>334080</xdr:rowOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>335520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>550800</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>315000</xdr:rowOff>
+      <xdr:colOff>550440</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>314640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2927,8 +2963,193 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9580680" y="21738600"/>
-          <a:ext cx="504360" cy="323640"/>
+          <a:off x="9966960" y="23263920"/>
+          <a:ext cx="504000" cy="322200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47160</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>7560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>361440</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>309240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="图片 30" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId58"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9967680" y="12199320"/>
+          <a:ext cx="314280" cy="301680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>46800</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>6120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>491040</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>338040</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="图片 29" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId59"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9967320" y="11436120"/>
+          <a:ext cx="444240" cy="331920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>46800</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>6840</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>491040</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>338760</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="图片 29" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId60"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9967320" y="12960720"/>
+          <a:ext cx="444240" cy="331920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>46800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>7560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>491040</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>339480</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="60" name="图片 29" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId61"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9967320" y="13342320"/>
+          <a:ext cx="444240" cy="331920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>46800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>7200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>491040</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>339120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="图片 29" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId62"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9967320" y="13723200"/>
+          <a:ext cx="444240" cy="331920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2950,18 +3171,18 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.60728744939271"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.96356275303644"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="35.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.49797570850202"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8380566801619"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="36.3117408906883"/>
     <col collapsed="false" hidden="false" max="20" min="7" style="1" width="8.03238866396761"/>
     <col collapsed="false" hidden="false" max="1020" min="21" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="9.10526315789474"/>
@@ -5064,7 +5285,7 @@
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="n">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>16</v>
@@ -9200,7 +9421,7 @@
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>28</v>
@@ -15402,7 +15623,7 @@
       <c r="AME13" s="0"/>
       <c r="AMF13" s="0"/>
     </row>
-    <row r="14" s="9" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="n">
         <v>1</v>
       </c>
@@ -15422,10 +15643,6 @@
         <v>50</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="AMG14" s="0"/>
-      <c r="AMH14" s="0"/>
-      <c r="AMI14" s="0"/>
-      <c r="AMJ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="n">
@@ -15759,7 +15976,7 @@
     </row>
     <row r="30" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>104</v>
@@ -15781,7 +15998,7 @@
     </row>
     <row r="31" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>107</v>
@@ -15803,59 +16020,59 @@
     </row>
     <row r="32" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>110</v>
       </c>
       <c r="C32" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G32" s="7"/>
       <c r="I32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>115</v>
+      <c r="D33" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G33" s="7"/>
       <c r="I33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="8" t="s">
         <v>118</v>
       </c>
       <c r="E34" s="6" t="s">
@@ -15877,7 +16094,7 @@
       <c r="C35" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="9" t="s">
         <v>121</v>
       </c>
       <c r="E35" s="6" t="s">
@@ -15899,7 +16116,7 @@
       <c r="C36" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="8" t="s">
         <v>124</v>
       </c>
       <c r="E36" s="6" t="s">
@@ -15913,15 +16130,15 @@
     </row>
     <row r="37" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>126</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D37" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E37" s="6" t="s">
@@ -15935,44 +16152,44 @@
     </row>
     <row r="38" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C38" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>131</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G38" s="7"/>
       <c r="I38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B39" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>135</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G39" s="7"/>
       <c r="I39" s="0"/>
@@ -15982,41 +16199,41 @@
         <v>1</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G40" s="7"/>
       <c r="I40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G41" s="7"/>
       <c r="I41" s="0"/>
@@ -16026,41 +16243,41 @@
         <v>1</v>
       </c>
       <c r="B42" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>143</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>145</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G42" s="7"/>
       <c r="I42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B43" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D43" s="11" t="s">
         <v>147</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>149</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G43" s="7"/>
       <c r="I43" s="0"/>
@@ -16070,19 +16287,19 @@
         <v>1</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G44" s="7"/>
       <c r="I44" s="0"/>
@@ -16092,19 +16309,19 @@
         <v>1</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>156</v>
+        <v>152</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>153</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>157</v>
+        <v>10</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G45" s="7"/>
       <c r="I45" s="0"/>
@@ -16114,63 +16331,63 @@
         <v>1</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>157</v>
+        <v>10</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G46" s="7"/>
       <c r="I46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G47" s="7"/>
       <c r="I47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B48" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>166</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G48" s="7"/>
       <c r="I48" s="0"/>
@@ -16180,19 +16397,19 @@
         <v>1</v>
       </c>
       <c r="B49" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="E49" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="F49" s="7" t="s">
         <v>170</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>171</v>
       </c>
       <c r="G49" s="7"/>
       <c r="I49" s="0"/>
@@ -16202,19 +16419,19 @@
         <v>1</v>
       </c>
       <c r="B50" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D50" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="E50" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="F50" s="7" t="s">
         <v>173</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>175</v>
       </c>
       <c r="G50" s="7"/>
       <c r="I50" s="0"/>
@@ -16224,41 +16441,41 @@
         <v>1</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G51" s="7"/>
       <c r="I51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B52" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D52" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>180</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G52" s="7"/>
       <c r="I52" s="0"/>
@@ -16268,132 +16485,220 @@
         <v>1</v>
       </c>
       <c r="B53" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D53" s="6" t="s">
         <v>182</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>184</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G53" s="7"/>
       <c r="I53" s="0"/>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0"/>
-      <c r="B54" s="0"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
+    <row r="54" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="G54" s="7"/>
       <c r="I54" s="0"/>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="14"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
+    <row r="55" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="G55" s="7"/>
       <c r="I55" s="0"/>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="B56" s="15"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="0"/>
-      <c r="F56" s="0"/>
-      <c r="G56" s="13"/>
+    <row r="56" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G56" s="7"/>
       <c r="I56" s="0"/>
     </row>
-    <row r="57" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="16" t="n">
-        <v>48</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="C57" s="15"/>
-      <c r="D57" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="E57" s="15" t="s">
+    <row r="57" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="E57" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F57" s="0"/>
-      <c r="G57" s="13"/>
-      <c r="I57" s="18" t="n">
-        <v>0.9</v>
-      </c>
+      <c r="F57" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="G57" s="7"/>
+      <c r="I57" s="0"/>
     </row>
-    <row r="58" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="B58" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="E58" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F58" s="0"/>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0"/>
+      <c r="B58" s="0"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="13"/>
       <c r="G58" s="13"/>
-      <c r="I58" s="18" t="n">
-        <v>59</v>
-      </c>
+      <c r="I58" s="0"/>
     </row>
-    <row r="59" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="B59" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="C59" s="15"/>
-      <c r="D59" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="E59" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F59" s="0"/>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="14"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="13"/>
       <c r="G59" s="13"/>
-      <c r="I59" s="18" t="n">
-        <v>55</v>
-      </c>
+      <c r="I59" s="0"/>
     </row>
-    <row r="60" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="B60" s="15" t="s">
-        <v>193</v>
-      </c>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="B60" s="15"/>
       <c r="C60" s="15"/>
-      <c r="D60" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="E60" s="15" t="s">
-        <v>10</v>
-      </c>
+      <c r="D60" s="15"/>
+      <c r="E60" s="0"/>
       <c r="F60" s="0"/>
       <c r="G60" s="13"/>
-      <c r="I60" s="18" t="n">
+      <c r="I60" s="0"/>
+    </row>
+    <row r="61" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="16" t="n">
+        <v>48</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="C61" s="15"/>
+      <c r="D61" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="E61" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" s="0"/>
+      <c r="G61" s="13"/>
+      <c r="I61" s="18" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="C62" s="15"/>
+      <c r="D62" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" s="0"/>
+      <c r="G62" s="13"/>
+      <c r="I62" s="18" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="C63" s="15"/>
+      <c r="D63" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" s="0"/>
+      <c r="G63" s="13"/>
+      <c r="I63" s="18" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="C64" s="15"/>
+      <c r="D64" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="E64" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" s="0"/>
+      <c r="G64" s="13"/>
+      <c r="I64" s="18" t="n">
         <v>98</v>
       </c>
     </row>

</xml_diff>